<commit_message>
Suivi du temps updated
</commit_message>
<xml_diff>
--- a/SuiviDuTemps.xlsx
+++ b/SuiviDuTemps.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -84,6 +84,12 @@
   </si>
   <si>
     <t>TitleScreen + Music + SFX</t>
+  </si>
+  <si>
+    <t>15/16-07-2015</t>
+  </si>
+  <si>
+    <t>EndScreen + polish + clean + proto done</t>
   </si>
 </sst>
 </file>
@@ -450,7 +456,7 @@
   <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,7 +566,15 @@
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D11" s="4"/>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="4">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D12" s="4"/>
@@ -610,7 +624,7 @@
       </c>
       <c r="D26" s="5">
         <f>SUM(D3:D25)</f>
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update suivi du temps
</commit_message>
<xml_diff>
--- a/SuiviDuTemps.xlsx
+++ b/SuiviDuTemps.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>Panel + hotfixes + musique</t>
+  </si>
+  <si>
+    <t>21-07-2015</t>
+  </si>
+  <si>
+    <t>Loc + musique + sfx</t>
   </si>
 </sst>
 </file>
@@ -462,7 +468,7 @@
   <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,7 +600,15 @@
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D13" s="4"/>
+      <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="4">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D14" s="4"/>
@@ -638,7 +652,7 @@
       </c>
       <c r="D26" s="5">
         <f>SUM(D3:D25)</f>
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remise 1 avec hotfixes done.
</commit_message>
<xml_diff>
--- a/SuiviDuTemps.xlsx
+++ b/SuiviDuTemps.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>Loc + musique + sfx</t>
+  </si>
+  <si>
+    <t>22-07-2015</t>
+  </si>
+  <si>
+    <t>Hotfixes</t>
   </si>
 </sst>
 </file>
@@ -468,7 +474,7 @@
   <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,7 +617,15 @@
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D14" s="4"/>
+      <c r="B14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D15" s="4"/>
@@ -652,7 +666,7 @@
       </c>
       <c r="D26" s="5">
         <f>SUM(D3:D25)</f>
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>